<commit_message>
Add P558-Lot Tools DP
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utaie\Desktop\Utai_Files\Delivery-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C60705B-4F7C-4F8E-B9F3-CDFE4774E143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8759B23-E268-406A-87E4-3F23B6BC6D93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="213">
   <si>
     <t>Component description</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Ingot-Typ</t>
   </si>
   <si>
-    <t>SCK-Cost</t>
-  </si>
-  <si>
     <t>5611011632A</t>
   </si>
   <si>
@@ -625,6 +622,57 @@
   </si>
   <si>
     <t>2300-0</t>
+  </si>
+  <si>
+    <t>T46496AA</t>
+  </si>
+  <si>
+    <t>CYLINDER HEAD (R) ,P558 V6</t>
+  </si>
+  <si>
+    <t>P558 V6</t>
+  </si>
+  <si>
+    <t>T46497AA</t>
+  </si>
+  <si>
+    <t>CYLINDER HEAD (R) ,P558 V8</t>
+  </si>
+  <si>
+    <t>P558 V8</t>
+  </si>
+  <si>
+    <t>T46511AB</t>
+  </si>
+  <si>
+    <t>T46515AB</t>
+  </si>
+  <si>
+    <t>6496</t>
+  </si>
+  <si>
+    <t>6497</t>
+  </si>
+  <si>
+    <t>6511</t>
+  </si>
+  <si>
+    <t>6515</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>ADC-13</t>
+  </si>
+  <si>
+    <t>ADC-15</t>
+  </si>
+  <si>
+    <t>ADC-16</t>
+  </si>
+  <si>
+    <t>MC-Cost</t>
   </si>
 </sst>
 </file>
@@ -664,12 +712,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -711,7 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -739,6 +793,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1078,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63:M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,10 +1159,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1125,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -1134,36 +1189,36 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>7</v>
+        <v>212</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="2">
         <v>171.9</v>
@@ -1172,23 +1227,23 @@
         <v>0.88200000000000001</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K2" s="2">
         <v>0</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N2" s="2">
         <v>0</v>
@@ -1197,21 +1252,21 @@
         <v>90</v>
       </c>
       <c r="P2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" s="2">
         <v>171.9</v>
@@ -1220,23 +1275,23 @@
         <v>0.88200000000000001</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K3" s="2">
         <v>0</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N3" s="2">
         <v>0</v>
@@ -1245,21 +1300,21 @@
         <v>90</v>
       </c>
       <c r="P3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E4" s="2">
         <v>287.70999999999998</v>
@@ -1268,23 +1323,23 @@
         <v>0.77</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K4" s="2">
         <v>0</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N4" s="2">
         <v>0</v>
@@ -1293,21 +1348,21 @@
         <v>90</v>
       </c>
       <c r="P4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="2">
         <v>288.70999999999998</v>
@@ -1316,23 +1371,23 @@
         <v>0.77</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N5" s="2">
         <v>0</v>
@@ -1341,21 +1396,21 @@
         <v>90</v>
       </c>
       <c r="P5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" s="2">
         <v>175.87</v>
@@ -1364,23 +1419,23 @@
         <v>0.89249999999999996</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K6" s="2">
         <v>0</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N6" s="2">
         <v>0</v>
@@ -1389,21 +1444,21 @@
         <v>90</v>
       </c>
       <c r="P6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" s="2">
         <v>173.08</v>
@@ -1412,23 +1467,23 @@
         <v>0.85575000000000001</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N7" s="2">
         <v>0</v>
@@ -1437,21 +1492,21 @@
         <v>90</v>
       </c>
       <c r="P7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="2">
         <v>186.46</v>
@@ -1460,23 +1515,23 @@
         <v>0.90300000000000002</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N8" s="2">
         <v>0</v>
@@ -1485,21 +1540,21 @@
         <v>90</v>
       </c>
       <c r="P8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E9" s="2">
         <v>183.71</v>
@@ -1508,23 +1563,23 @@
         <v>0.86099999999999999</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N9" s="2">
         <v>0</v>
@@ -1533,21 +1588,21 @@
         <v>90</v>
       </c>
       <c r="P9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E10" s="2">
         <v>185.4</v>
@@ -1556,23 +1611,23 @@
         <v>0.88200000000000001</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
       </c>
       <c r="L10" s="2"/>
       <c r="M10" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N10" s="2">
         <v>0</v>
@@ -1581,21 +1636,21 @@
         <v>90</v>
       </c>
       <c r="P10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11" s="2">
         <v>182.69</v>
@@ -1604,23 +1659,23 @@
         <v>0.86099999999999999</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N11" s="2">
         <v>0</v>
@@ -1629,21 +1684,21 @@
         <v>90</v>
       </c>
       <c r="P11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E12" s="2">
         <v>182.59</v>
@@ -1652,23 +1707,23 @@
         <v>0.86099999999999999</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N12" s="2">
         <v>0</v>
@@ -1677,21 +1732,21 @@
         <v>90</v>
       </c>
       <c r="P12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E13" s="2">
         <v>196.04</v>
@@ -1700,23 +1755,23 @@
         <v>1.008</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
@@ -1725,21 +1780,21 @@
         <v>90</v>
       </c>
       <c r="P13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E14" s="2">
         <v>196.15</v>
@@ -1748,23 +1803,23 @@
         <v>1.008</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K14" s="2">
         <v>0</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N14" s="2">
         <v>0</v>
@@ -1773,21 +1828,21 @@
         <v>90</v>
       </c>
       <c r="P14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E15" s="2">
         <v>182.93</v>
@@ -1796,23 +1851,23 @@
         <v>0.99750000000000005</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K15" s="2">
         <v>0</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N15" s="2">
         <v>0</v>
@@ -1821,21 +1876,21 @@
         <v>90</v>
       </c>
       <c r="P15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E16" s="2">
         <v>181.43</v>
@@ -1844,23 +1899,23 @@
         <v>0.98699999999999999</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K16" s="2">
         <v>0</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N16" s="2">
         <v>0</v>
@@ -1869,21 +1924,21 @@
         <v>90</v>
       </c>
       <c r="P16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E17" s="2">
         <v>181.55</v>
@@ -1892,23 +1947,23 @@
         <v>0.99750000000000005</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K17" s="2">
         <v>0</v>
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N17" s="2">
         <v>0</v>
@@ -1917,21 +1972,21 @@
         <v>90</v>
       </c>
       <c r="P17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E18" s="2">
         <v>130.41</v>
@@ -1940,23 +1995,23 @@
         <v>0.41265000000000002</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K18" s="2">
         <v>30</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N18" s="2">
         <v>0</v>
@@ -1965,21 +2020,21 @@
         <v>90</v>
       </c>
       <c r="P18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
@@ -1988,46 +2043,46 @@
         <v>0</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K19" s="2">
         <v>0</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O19" s="9">
         <v>90</v>
       </c>
       <c r="P19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="2">
         <v>131.61000000000001</v>
@@ -2036,46 +2091,46 @@
         <v>0.42</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K20" s="2">
         <v>30</v>
       </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N20" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N20" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O20" s="9">
         <v>90</v>
       </c>
       <c r="P20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E21" s="2">
         <v>142.44999999999999</v>
@@ -2084,46 +2139,46 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K21" s="2">
         <v>30</v>
       </c>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O21" s="9">
         <v>90</v>
       </c>
       <c r="P21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" s="2">
         <v>143.21</v>
@@ -2132,46 +2187,46 @@
         <v>0.441</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K22" s="2">
         <v>30</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O22" s="9">
         <v>90</v>
       </c>
       <c r="P22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E23" s="2">
         <v>158.21</v>
@@ -2180,23 +2235,23 @@
         <v>0.441</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K23" s="2">
         <v>30</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N23" s="2">
         <v>0</v>
@@ -2205,21 +2260,21 @@
         <v>90</v>
       </c>
       <c r="P23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E24" s="2">
         <v>142.44999999999999</v>
@@ -2228,23 +2283,23 @@
         <v>0.48299999999999998</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K24" s="2">
         <v>30</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N24" s="2">
         <v>0</v>
@@ -2253,21 +2308,21 @@
         <v>90</v>
       </c>
       <c r="P24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E25" s="2">
         <v>148.30000000000001</v>
@@ -2276,46 +2331,46 @@
         <v>0.441</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K25" s="2">
         <v>30</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N25" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N25" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O25" s="9">
         <v>90</v>
       </c>
       <c r="P25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E26" s="2">
         <v>167.91</v>
@@ -2324,46 +2379,46 @@
         <v>0.441</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K26" s="2">
         <v>30</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N26" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N26" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O26" s="9">
         <v>90</v>
       </c>
       <c r="P26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E27" s="2">
         <v>157.30000000000001</v>
@@ -2372,46 +2427,46 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K27" s="2">
         <v>30</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O27" s="9">
         <v>90</v>
       </c>
       <c r="P27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
@@ -2420,46 +2475,46 @@
         <v>0.41265000000000002</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K28" s="2">
         <v>0</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O28" s="9">
         <v>90</v>
       </c>
       <c r="P28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E29" s="2">
         <v>148.51</v>
@@ -2468,46 +2523,46 @@
         <v>0.441</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K29" s="2">
         <v>30</v>
       </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O29" s="9">
         <v>90</v>
       </c>
       <c r="P29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
@@ -2516,46 +2571,46 @@
         <v>0</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K30" s="2">
         <v>0</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N30" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N30" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O30" s="9">
         <v>90</v>
       </c>
       <c r="P30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E31" s="2">
         <v>136.13999999999999</v>
@@ -2564,46 +2619,46 @@
         <v>0.41265000000000002</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K31" s="2">
         <v>30</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O31" s="9">
         <v>90</v>
       </c>
       <c r="P31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E32" s="2">
         <v>142.78</v>
@@ -2612,23 +2667,23 @@
         <v>0.36749999999999999</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K32" s="2">
         <v>45</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N32" s="2">
         <v>0</v>
@@ -2637,21 +2692,21 @@
         <v>90</v>
       </c>
       <c r="P32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E33" s="2">
         <v>195.22</v>
@@ -2660,23 +2715,23 @@
         <v>0.71399999999999997</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K33" s="2">
         <v>45</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N33" s="2">
         <v>0</v>
@@ -2685,21 +2740,21 @@
         <v>90</v>
       </c>
       <c r="P33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E34" s="2">
         <v>194.71</v>
@@ -2708,23 +2763,23 @@
         <v>0.78</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K34" s="2">
         <v>0</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N34" s="2">
         <v>0</v>
@@ -2733,22 +2788,22 @@
         <v>90</v>
       </c>
       <c r="P34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q34" s="16"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35" s="2">
         <v>184.56</v>
@@ -2757,23 +2812,23 @@
         <v>0.66</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K35" s="2">
         <v>0</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N35" s="2">
         <v>0</v>
@@ -2782,21 +2837,21 @@
         <v>90</v>
       </c>
       <c r="P35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E36" s="2">
         <v>208.99</v>
@@ -2805,23 +2860,23 @@
         <v>0.74550000000000005</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K36" s="2">
         <v>45</v>
       </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N36" s="2">
         <v>0</v>
@@ -2830,21 +2885,21 @@
         <v>90</v>
       </c>
       <c r="P36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E37" s="2">
         <v>198.13</v>
@@ -2853,23 +2908,23 @@
         <v>0.74760000000000004</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K37" s="2">
         <v>45</v>
       </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N37" s="2">
         <v>0</v>
@@ -2878,21 +2933,21 @@
         <v>90</v>
       </c>
       <c r="P37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E38" s="2">
         <v>312.70999999999998</v>
@@ -2901,23 +2956,23 @@
         <v>0.59</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K38" s="2">
         <v>0</v>
       </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N38" s="2">
         <v>0</v>
@@ -2926,21 +2981,21 @@
         <v>90</v>
       </c>
       <c r="P38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E39" s="2">
         <v>356.71</v>
@@ -2949,23 +3004,23 @@
         <v>0.76</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K39" s="2">
         <v>0</v>
       </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N39" s="2">
         <v>0</v>
@@ -2974,21 +3029,21 @@
         <v>90</v>
       </c>
       <c r="P39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E40" s="2">
         <v>218.45</v>
@@ -2997,23 +3052,23 @@
         <v>0.89</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K40" s="2">
         <v>0</v>
       </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N40" s="2">
         <v>0</v>
@@ -3022,21 +3077,21 @@
         <v>90</v>
       </c>
       <c r="P40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E41" s="2">
         <v>165.02</v>
@@ -3045,23 +3100,23 @@
         <v>0.47249999999999998</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K41" s="2">
         <v>45</v>
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N41" s="2">
         <v>0</v>
@@ -3070,21 +3125,21 @@
         <v>90</v>
       </c>
       <c r="P41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E42" s="2">
         <v>141.81</v>
@@ -3093,46 +3148,46 @@
         <v>0.65100000000000002</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K42" s="2">
         <v>0</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N42" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N42" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O42" s="9">
         <v>90</v>
       </c>
       <c r="P42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E43" s="2">
         <v>195.25</v>
@@ -3141,46 +3196,46 @@
         <v>0.66149999999999998</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K43" s="2">
         <v>0</v>
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N43" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N43" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O43" s="9">
         <v>90</v>
       </c>
       <c r="P43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E44" s="2">
         <v>142.66999999999999</v>
@@ -3189,23 +3244,23 @@
         <v>0.66149999999999998</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K44" s="2">
         <v>0</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N44" s="2">
         <v>0</v>
@@ -3214,21 +3269,21 @@
         <v>90</v>
       </c>
       <c r="P44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E45" s="2">
         <v>133.06</v>
@@ -3237,23 +3292,23 @@
         <v>0.54600000000000004</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K45" s="2">
         <v>0</v>
       </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N45" s="2">
         <v>0</v>
@@ -3262,21 +3317,21 @@
         <v>90</v>
       </c>
       <c r="P45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E46" s="2">
         <v>223.71</v>
@@ -3285,23 +3340,23 @@
         <v>0.64049999999999996</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K46" s="2">
         <v>50</v>
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N46" s="2">
         <v>0</v>
@@ -3310,21 +3365,21 @@
         <v>90</v>
       </c>
       <c r="P46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E47" s="2">
         <v>137.82</v>
@@ -3333,23 +3388,23 @@
         <v>0.56699999999999995</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K47" s="2">
         <v>0</v>
       </c>
       <c r="L47" s="2"/>
       <c r="M47" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N47" s="2">
         <v>0</v>
@@ -3358,21 +3413,21 @@
         <v>90</v>
       </c>
       <c r="P47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E48" s="2">
         <v>148.88999999999999</v>
@@ -3381,46 +3436,46 @@
         <v>0.53549999999999998</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K48" s="2">
         <v>0</v>
       </c>
       <c r="L48" s="2"/>
       <c r="M48" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N48" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O48" s="9">
         <v>90</v>
       </c>
       <c r="P48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E49" s="2">
         <v>164.93</v>
@@ -3429,46 +3484,46 @@
         <v>0.77070000000000005</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K49" s="2">
         <v>0</v>
       </c>
       <c r="L49" s="2"/>
       <c r="M49" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N49" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N49" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O49" s="9">
         <v>90</v>
       </c>
       <c r="P49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E50" s="2">
         <v>166.24</v>
@@ -3477,46 +3532,46 @@
         <v>0.79064999999999996</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K50" s="2">
         <v>0</v>
       </c>
       <c r="L50" s="2"/>
       <c r="M50" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N50" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N50" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O50" s="9">
         <v>90</v>
       </c>
       <c r="P50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E51" s="2">
         <v>177.41</v>
@@ -3525,46 +3580,46 @@
         <v>0.53549999999999998</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K51" s="2">
         <v>0</v>
       </c>
       <c r="L51" s="2"/>
       <c r="M51" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N51" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O51" s="9">
         <v>90</v>
       </c>
       <c r="P51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="3">
         <v>5400</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E52" s="4">
         <v>0</v>
@@ -3573,46 +3628,46 @@
         <v>0</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K52" s="2">
         <v>0</v>
       </c>
       <c r="L52" s="2"/>
       <c r="M52" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N52" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N52" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O52" s="9">
         <v>90</v>
       </c>
       <c r="P52" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="3">
         <v>5501</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E53" s="4">
         <v>0</v>
@@ -3621,46 +3676,46 @@
         <v>0</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K53" s="2">
         <v>0</v>
       </c>
       <c r="L53" s="2"/>
       <c r="M53" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N53" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N53" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O53" s="9">
         <v>90</v>
       </c>
       <c r="P53" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E54" s="4">
         <v>0</v>
@@ -3669,46 +3724,46 @@
         <v>0</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K54" s="2">
         <v>0</v>
       </c>
       <c r="L54" s="2"/>
       <c r="M54" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N54" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N54" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O54" s="9">
         <v>90</v>
       </c>
       <c r="P54" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E55" s="4">
         <v>0</v>
@@ -3717,46 +3772,46 @@
         <v>0</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K55" s="2">
         <v>0</v>
       </c>
       <c r="L55" s="2"/>
       <c r="M55" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N55" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N55" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O55" s="9">
         <v>90</v>
       </c>
       <c r="P55" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E56" s="4">
         <v>0</v>
@@ -3765,92 +3820,92 @@
         <v>0</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K56" s="2">
         <v>0</v>
       </c>
       <c r="L56" s="2"/>
       <c r="M56" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N56" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="N56" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="O56" s="9">
         <v>90</v>
       </c>
       <c r="P56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="2">
         <v>0</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K57" s="2">
         <v>0</v>
       </c>
       <c r="L57" s="2"/>
       <c r="M57" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N57" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O57" s="9">
         <v>90</v>
       </c>
       <c r="P57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E58" s="4">
         <v>136.63999999999999</v>
@@ -3859,23 +3914,23 @@
         <v>0</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K58" s="2">
         <v>0</v>
       </c>
       <c r="L58" s="2"/>
       <c r="M58" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N58" s="2">
         <v>0</v>
@@ -3884,21 +3939,21 @@
         <v>90</v>
       </c>
       <c r="P58" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E59" s="4">
         <v>88.41</v>
@@ -3907,23 +3962,23 @@
         <v>0</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K59" s="2">
         <v>0</v>
       </c>
       <c r="L59" s="2"/>
       <c r="M59" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N59" s="2">
         <v>0</v>
@@ -3932,21 +3987,21 @@
         <v>90</v>
       </c>
       <c r="P59" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E60" s="4">
         <v>94.54</v>
@@ -3955,23 +4010,23 @@
         <v>0</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K60" s="2">
         <v>0</v>
       </c>
       <c r="L60" s="2"/>
       <c r="M60" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N60" s="2">
         <v>0</v>
@@ -3980,21 +4035,21 @@
         <v>90</v>
       </c>
       <c r="P60" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E61" s="4">
         <v>150</v>
@@ -4003,23 +4058,23 @@
         <v>0</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K61" s="2">
         <v>0</v>
       </c>
       <c r="L61" s="2"/>
       <c r="M61" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N61" s="2">
         <v>0</v>
@@ -4028,21 +4083,21 @@
         <v>90</v>
       </c>
       <c r="P61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E62" s="4">
         <v>150</v>
@@ -4051,23 +4106,23 @@
         <v>0</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K62" s="2">
         <v>0</v>
       </c>
       <c r="L62" s="2"/>
       <c r="M62" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N62" s="2">
         <v>0</v>
@@ -4076,125 +4131,273 @@
         <v>90</v>
       </c>
       <c r="P62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E63" s="17">
+        <v>542.89</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H63" s="11"/>
+      <c r="I63" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K63" s="2">
+        <v>180</v>
+      </c>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N63" s="2"/>
+      <c r="O63" s="9"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" s="17">
+        <v>542.89</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H64" s="11"/>
+      <c r="I64" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K64" s="2">
+        <v>180</v>
+      </c>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N64" s="2"/>
+      <c r="O64" s="9"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E65" s="17">
+        <v>430.95</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H65" s="11"/>
+      <c r="I65" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K65" s="2">
+        <v>0</v>
+      </c>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N65" s="2"/>
+      <c r="O65" s="9"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E66" s="17">
+        <v>430.95</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H66" s="11"/>
+      <c r="I66" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="K66" s="2">
+        <v>0</v>
+      </c>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N66" s="2"/>
+      <c r="O66" s="9"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B67" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="B63" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="C63" s="7" t="s">
+      <c r="C67" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E67" s="15">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K67" s="14">
+        <v>2</v>
+      </c>
+      <c r="L67" s="14">
+        <v>2.4</v>
+      </c>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D68" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E68" s="15">
+        <v>9</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="G68" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H68" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E63" s="15">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="F63" s="2"/>
-      <c r="G63" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="H63" s="13" t="s">
+      <c r="I68" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="I63" s="7" t="s">
+      <c r="J68" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="J63" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="K63" s="14">
+      <c r="K68" s="14">
         <v>2</v>
       </c>
-      <c r="L63" s="14">
+      <c r="L68" s="14">
         <v>2.4</v>
       </c>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B64" s="12" t="s">
+      <c r="B69" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C69" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D69" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69" s="15">
+        <v>8</v>
+      </c>
+      <c r="F69" s="2"/>
+      <c r="G69" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H69" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E64" s="15">
-        <v>9</v>
-      </c>
-      <c r="F64" s="2"/>
-      <c r="G64" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="H64" s="13" t="s">
+      <c r="I69" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="J69" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="J64" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="K64" s="14">
+      <c r="K69" s="14">
         <v>2</v>
       </c>
-      <c r="L64" s="14">
+      <c r="L69" s="14">
         <v>2.4</v>
       </c>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E65" s="15">
-        <v>8</v>
-      </c>
-      <c r="F65" s="2"/>
-      <c r="G65" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="H65" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="I65" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="J65" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="K65" s="14">
-        <v>2</v>
-      </c>
-      <c r="L65" s="14">
-        <v>2.4</v>
-      </c>
-      <c r="M65" s="2"/>
-      <c r="N65" s="2"/>
-      <c r="O65" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>